<commit_message>
Updated unit tests statistics.
</commit_message>
<xml_diff>
--- a/ParserTest/ResultDocuments/Unit tests.xlsx
+++ b/ParserTest/ResultDocuments/Unit tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>AngleSharpParser</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Passing rate</t>
   </si>
   <si>
-    <t>Incorrect encoding detection</t>
-  </si>
-  <si>
     <t>Problems</t>
   </si>
   <si>
@@ -51,12 +48,6 @@
     <t>&lt; 2 sec</t>
   </si>
   <si>
-    <t>Slow, incorrect encoding detection</t>
-  </si>
-  <si>
-    <t>Not working</t>
-  </si>
-  <si>
     <t>doc</t>
   </si>
   <si>
@@ -100,6 +91,9 @@
   </si>
   <si>
     <t>&gt; 26 min</t>
+  </si>
+  <si>
+    <t>Slow</t>
   </si>
 </sst>
 </file>
@@ -213,13 +207,13 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="0.00%">
-                  <c:v>0.8125</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00%">
-                  <c:v>0.375</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.94</c:v>
@@ -606,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -630,10 +624,10 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -644,114 +638,108 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>0.8125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
-        <v>0.75</v>
+        <v>0.93</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
-        <v>0.375</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2">
         <v>0.94</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2">
         <v>0.94</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1">
         <v>0.76500000000000001</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2">
         <v>0.93</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2">
         <v>0.73</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>